<commit_message>
Updated and made new rubrics
</commit_message>
<xml_diff>
--- a/Labs/Lab05/Lab5Rubric_CS295N.xlsx
+++ b/Labs/Lab05/Lab5Rubric_CS295N.xlsx
@@ -5,36 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS295N-CourseMaterials/Labs/Lab05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C264AAA7-012D-CE42-9331-AF640886B176}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBF281C-6C6E-9A48-AA1E-1D5F57664DE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36260" yWindow="9640" windowWidth="23520" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28120" yWindow="8960" windowWidth="10000" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab3Rubric_CS295N" sheetId="1" r:id="rId1"/>
+    <sheet name="Student Points" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
-  <si>
-    <t>Lab 3, Group A - Community Web Site</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>-----------------------------------</t>
-  </si>
-  <si>
-    <t>Excellent work! Everything looks great!</t>
-  </si>
-  <si>
-    <t>Coding style and best practices: 4/4</t>
-  </si>
-  <si>
-    <t>Code review by lab partner: 1/1</t>
   </si>
   <si>
     <t>Actual</t>
@@ -43,92 +32,29 @@
     <t>Possible</t>
   </si>
   <si>
-    <t>1. Contact page</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>2. Location + People pages</t>
-  </si>
-  <si>
-    <t>3. Code Quality</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Lab 3, Group B - Fan Site</t>
+    <t>Lab 5, Both Groups</t>
   </si>
   <si>
-    <t>1. Stories page</t>
+    <t>App is running correctly (with no database)</t>
   </si>
   <si>
-    <t>Comment controller methods</t>
+    <t>Deploy to a web server</t>
   </si>
   <si>
-    <t>Comment view(s)</t>
+    <t>Register a domain name</t>
   </si>
   <si>
-    <t>Sort stories with lambda</t>
-  </si>
-  <si>
-    <t>repo refactor if needed</t>
-  </si>
-  <si>
-    <t>XC: story rating</t>
-  </si>
-  <si>
-    <t>2. Books and Print Media, Online Media pages</t>
-  </si>
-  <si>
-    <t>Print media table in view from data</t>
-  </si>
-  <si>
-    <t>Online media view table from data</t>
-  </si>
-  <si>
-    <t>Sort print media with lambda</t>
-  </si>
-  <si>
-    <t>Sort online media with lambda</t>
-  </si>
-  <si>
-    <t>Coding style and best practices</t>
-  </si>
-  <si>
-    <t>Code review by lab partner</t>
-  </si>
-  <si>
-    <t>reply controller methods</t>
-  </si>
-  <si>
-    <t>reply view(s)</t>
-  </si>
-  <si>
-    <t>Sort messages with lambda</t>
-  </si>
-  <si>
-    <t>XC: message priority</t>
-  </si>
-  <si>
-    <t>Location table from data</t>
-  </si>
-  <si>
-    <t>People table from data</t>
-  </si>
-  <si>
-    <t>Sort locations with lambda</t>
-  </si>
-  <si>
-    <t>Sort people with lambda</t>
+    <t>Excellent work! Your web site works! </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -278,6 +204,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
     </font>
   </fonts>
   <fills count="33">
@@ -621,7 +558,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -632,6 +569,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,449 +926,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:C50"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="19">
       <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <f>SUM(B6:B8)</f>
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <f>SUM(C6:C8)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="48" spans="1:3" s="4" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5E9A37-39B4-9C4E-A961-C4057A6293B3}">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3">
-        <f>SUM(B6:B10)</f>
-        <v>28</v>
-      </c>
-      <c r="C11" s="3">
-        <f>SUM(C6:C9)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3">
-        <f>SUM(B14:B17)</f>
-        <v>22</v>
-      </c>
-      <c r="C18" s="3">
-        <f>SUM(C14:C17)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3">
-        <f>SUM(C21:C22)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="4">
-        <f>SUM(B11,B18,B23)</f>
+      <c r="B9" s="3">
+        <f>SUM(B6:B8)</f>
         <v>50</v>
       </c>
-      <c r="C25" s="4">
-        <f>SUM(C11,C18,C23)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="3">
-        <f>SUM(B31:B35)</f>
-        <v>23</v>
-      </c>
-      <c r="C36" s="3">
-        <f>SUM(C31:C34)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="C9" s="3">
+        <f>SUM(C6:C8)</f>
         <v>20</v>
       </c>
-      <c r="B39">
-        <v>8</v>
-      </c>
-      <c r="C39">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40">
-        <v>8</v>
-      </c>
-      <c r="C40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="3">
-        <f>SUM(B39:B42)</f>
-        <v>22</v>
-      </c>
-      <c r="C43" s="3">
-        <f>SUM(C39:C42)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="3">
-        <f>SUM(B46:B47)</f>
-        <v>5</v>
-      </c>
-      <c r="C48" s="3">
-        <f>SUM(C46:C47)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="4">
-        <f>SUM(B36,B43,B48)</f>
-        <v>50</v>
-      </c>
-      <c r="C50" s="4">
-        <f>SUM(C36,C43,C48)</f>
-        <v>50</v>
-      </c>
-    </row>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="48" spans="1:3" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>